<commit_message>
Se encontro un error en escenarios Infl
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_INF_Demand.xlsx
+++ b/SuppXLS/Scen_INF_Demand.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD3FF0A-01AB-4C02-90C7-DC85C7A2C7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009ECE98-D98B-4991-9E6F-1A44181F534F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25920" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEM_Especifica" sheetId="1" r:id="rId1"/>
-    <sheet name="DEM_General" sheetId="2" r:id="rId2"/>
+    <sheet name="datos" sheetId="3" r:id="rId2"/>
+    <sheet name="DEM_General" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="61">
   <si>
     <t>TechName</t>
   </si>
@@ -1158,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AE288"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28:N33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10032,6 +10033,1114 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9DC9D-38B5-4D3B-BABA-1E63DDFBA5A1}">
+  <dimension ref="D8:P36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:P36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D8" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="59">
+        <v>1</v>
+      </c>
+      <c r="I8" s="45">
+        <v>0.70492284759636947</v>
+      </c>
+      <c r="J8" s="46">
+        <v>0.71027709227023539</v>
+      </c>
+      <c r="K8" s="46">
+        <v>0.71018283052707665</v>
+      </c>
+      <c r="L8" s="46">
+        <v>0.71320579170785603</v>
+      </c>
+      <c r="M8" s="46">
+        <v>0.71486629778146171</v>
+      </c>
+      <c r="N8" s="46">
+        <v>0.71503401741990957</v>
+      </c>
+      <c r="O8" s="46">
+        <v>0.71399693928190033</v>
+      </c>
+      <c r="P8" s="47">
+        <v>0.71196823116894092</v>
+      </c>
+    </row>
+    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D9" s="60"/>
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="23">
+        <v>1</v>
+      </c>
+      <c r="I9" s="25">
+        <v>6.6022474682462001E-2</v>
+      </c>
+      <c r="J9" s="26">
+        <v>6.6523948687212134E-2</v>
+      </c>
+      <c r="K9" s="26">
+        <v>6.651512021247559E-2</v>
+      </c>
+      <c r="L9" s="26">
+        <v>6.6798248186983156E-2</v>
+      </c>
+      <c r="M9" s="26">
+        <v>6.6953769774315053E-2</v>
+      </c>
+      <c r="N9" s="26">
+        <v>6.6969478253081111E-2</v>
+      </c>
+      <c r="O9" s="26">
+        <v>6.6872346396248949E-2</v>
+      </c>
+      <c r="P9" s="48">
+        <v>6.6682339318903286E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D10" s="60"/>
+      <c r="E10" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="43">
+        <v>1</v>
+      </c>
+      <c r="I10" s="49">
+        <v>6.6920156894449958E-3</v>
+      </c>
+      <c r="J10" s="50">
+        <v>6.929791145634928E-3</v>
+      </c>
+      <c r="K10" s="50">
+        <v>6.77249243782959E-3</v>
+      </c>
+      <c r="L10" s="50">
+        <v>6.6178805784550977E-3</v>
+      </c>
+      <c r="M10" s="50">
+        <v>6.5021617867783779E-3</v>
+      </c>
+      <c r="N10" s="50">
+        <v>6.4218783098451155E-3</v>
+      </c>
+      <c r="O10" s="50">
+        <v>6.3682683038996874E-3</v>
+      </c>
+      <c r="P10" s="51">
+        <v>6.3368678974272319E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D11" s="60"/>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="23">
+        <v>1</v>
+      </c>
+      <c r="I11" s="25">
+        <v>3.8560214180194803E-4</v>
+      </c>
+      <c r="J11" s="26">
+        <v>3.9930305486456775E-4</v>
+      </c>
+      <c r="K11" s="26">
+        <v>3.9023931062856949E-4</v>
+      </c>
+      <c r="L11" s="26">
+        <v>3.8133038589056872E-4</v>
+      </c>
+      <c r="M11" s="26">
+        <v>3.7466252735765223E-4</v>
+      </c>
+      <c r="N11" s="26">
+        <v>3.7003649506881571E-4</v>
+      </c>
+      <c r="O11" s="26">
+        <v>3.6694742085352695E-4</v>
+      </c>
+      <c r="P11" s="48">
+        <v>3.6513809096681913E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D12" s="61"/>
+      <c r="E12" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="65">
+        <v>1</v>
+      </c>
+      <c r="I12" s="52">
+        <v>0.28838513671418559</v>
+      </c>
+      <c r="J12" s="53">
+        <v>0.28279311658412976</v>
+      </c>
+      <c r="K12" s="53">
+        <v>0.28304467703509384</v>
+      </c>
+      <c r="L12" s="53">
+        <v>0.28017632771368889</v>
+      </c>
+      <c r="M12" s="53">
+        <v>0.27863154043175997</v>
+      </c>
+      <c r="N12" s="53">
+        <v>0.27854410427024534</v>
+      </c>
+      <c r="O12" s="53">
+        <v>0.27963479241419981</v>
+      </c>
+      <c r="P12" s="54">
+        <v>0.28169490093363186</v>
+      </c>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D13" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="59">
+        <v>1</v>
+      </c>
+      <c r="I13" s="45">
+        <v>0.94914717262718429</v>
+      </c>
+      <c r="J13" s="46">
+        <v>0.94900036088054851</v>
+      </c>
+      <c r="K13" s="46">
+        <v>0.94207287924935468</v>
+      </c>
+      <c r="L13" s="46">
+        <v>0.93664116240507755</v>
+      </c>
+      <c r="M13" s="46">
+        <v>0.96537160286355184</v>
+      </c>
+      <c r="N13" s="46">
+        <v>0.99584958281549263</v>
+      </c>
+      <c r="O13" s="46">
+        <v>0.99970556052374615</v>
+      </c>
+      <c r="P13" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D14" s="61"/>
+      <c r="E14" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="63"/>
+      <c r="G14" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="65">
+        <v>1</v>
+      </c>
+      <c r="I14" s="52">
+        <v>5.0852827372815664E-2</v>
+      </c>
+      <c r="J14" s="53">
+        <v>5.0999639119451462E-2</v>
+      </c>
+      <c r="K14" s="53">
+        <v>5.7927120750645336E-2</v>
+      </c>
+      <c r="L14" s="53">
+        <v>6.335883759492239E-2</v>
+      </c>
+      <c r="M14" s="53">
+        <v>3.4628397136448101E-2</v>
+      </c>
+      <c r="N14" s="53">
+        <v>4.150417184507307E-3</v>
+      </c>
+      <c r="O14" s="53">
+        <v>2.9443947625379857E-4</v>
+      </c>
+      <c r="P14" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="59">
+        <v>1</v>
+      </c>
+      <c r="I15" s="45">
+        <v>0.73862618670258562</v>
+      </c>
+      <c r="J15" s="46">
+        <v>0.73892113329867415</v>
+      </c>
+      <c r="K15" s="46">
+        <v>0.74889110966438177</v>
+      </c>
+      <c r="L15" s="46">
+        <v>0.74775912300544867</v>
+      </c>
+      <c r="M15" s="46">
+        <v>0.73576050160718331</v>
+      </c>
+      <c r="N15" s="46">
+        <v>0.70077220806192775</v>
+      </c>
+      <c r="O15" s="46">
+        <v>0.48247290434054141</v>
+      </c>
+      <c r="P15" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="61"/>
+      <c r="E16" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="63"/>
+      <c r="G16" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="65">
+        <v>1</v>
+      </c>
+      <c r="I16" s="52">
+        <v>0.26137381329741433</v>
+      </c>
+      <c r="J16" s="53">
+        <v>0.26107886670132585</v>
+      </c>
+      <c r="K16" s="53">
+        <v>0.25110889033561812</v>
+      </c>
+      <c r="L16" s="53">
+        <v>0.25224087699455128</v>
+      </c>
+      <c r="M16" s="53">
+        <v>0.26423949839281657</v>
+      </c>
+      <c r="N16" s="53">
+        <v>0.29922779193807231</v>
+      </c>
+      <c r="O16" s="53">
+        <v>0.51752709565945865</v>
+      </c>
+      <c r="P16" s="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D17" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="59">
+        <v>1</v>
+      </c>
+      <c r="I17" s="45">
+        <v>2.3815208477444158E-2</v>
+      </c>
+      <c r="J17" s="46">
+        <v>2.2291811973852816E-2</v>
+      </c>
+      <c r="K17" s="46">
+        <v>1.8488966144340289E-2</v>
+      </c>
+      <c r="L17" s="46">
+        <v>1.3679255515304019E-2</v>
+      </c>
+      <c r="M17" s="46">
+        <v>9.258820007557551E-3</v>
+      </c>
+      <c r="N17" s="46">
+        <v>5.3838956440186592E-3</v>
+      </c>
+      <c r="O17" s="46">
+        <v>3.4997362435408037E-3</v>
+      </c>
+      <c r="P17" s="47">
+        <v>1.6243768554304598E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D18" s="60"/>
+      <c r="E18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="23">
+        <v>1</v>
+      </c>
+      <c r="I18" s="25">
+        <v>2.230512181752852E-3</v>
+      </c>
+      <c r="J18" s="26">
+        <v>2.0878321601977834E-3</v>
+      </c>
+      <c r="K18" s="26">
+        <v>1.7316608524349532E-3</v>
+      </c>
+      <c r="L18" s="26">
+        <v>1.2811874434395048E-3</v>
+      </c>
+      <c r="M18" s="26">
+        <v>8.6717321139867303E-4</v>
+      </c>
+      <c r="N18" s="26">
+        <v>5.042510894096747E-4</v>
+      </c>
+      <c r="O18" s="26">
+        <v>3.2778232160063326E-4</v>
+      </c>
+      <c r="P18" s="48">
+        <v>1.5213775546943573E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D19" s="60"/>
+      <c r="E19" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="43">
+        <v>1</v>
+      </c>
+      <c r="I19" s="49">
+        <v>2.0733084888629265E-3</v>
+      </c>
+      <c r="J19" s="50">
+        <v>4.6156996642390223E-3</v>
+      </c>
+      <c r="K19" s="50">
+        <v>4.1776372247926703E-3</v>
+      </c>
+      <c r="L19" s="50">
+        <v>3.3657996919672878E-3</v>
+      </c>
+      <c r="M19" s="50">
+        <v>2.610790942060398E-3</v>
+      </c>
+      <c r="N19" s="50">
+        <v>2.14961401171441E-3</v>
+      </c>
+      <c r="O19" s="50">
+        <v>2.1258077344612158E-3</v>
+      </c>
+      <c r="P19" s="51">
+        <v>2.0961786211324105E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="60"/>
+      <c r="E20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="23">
+        <v>1</v>
+      </c>
+      <c r="I20" s="25">
+        <v>1.1946657494881176E-4</v>
+      </c>
+      <c r="J20" s="26">
+        <v>2.6596226892479228E-4</v>
+      </c>
+      <c r="K20" s="26">
+        <v>2.4072057453367998E-4</v>
+      </c>
+      <c r="L20" s="26">
+        <v>1.9394150138439997E-4</v>
+      </c>
+      <c r="M20" s="26">
+        <v>1.5043697232262589E-4</v>
+      </c>
+      <c r="N20" s="26">
+        <v>1.2386339265042863E-4</v>
+      </c>
+      <c r="O20" s="26">
+        <v>1.2249164579220749E-4</v>
+      </c>
+      <c r="P20" s="48">
+        <v>1.2078437998628593E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D21" s="60"/>
+      <c r="E21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="43">
+        <v>1</v>
+      </c>
+      <c r="I21" s="49">
+        <v>0.92987932910492899</v>
+      </c>
+      <c r="J21" s="50">
+        <v>0.92789147783490933</v>
+      </c>
+      <c r="K21" s="50">
+        <v>0.93587746814734207</v>
+      </c>
+      <c r="L21" s="50">
+        <v>0.94391982472504832</v>
+      </c>
+      <c r="M21" s="50">
+        <v>0.95160712503823763</v>
+      </c>
+      <c r="N21" s="50">
+        <v>0.95939252769919714</v>
+      </c>
+      <c r="O21" s="50">
+        <v>0.9647057933775387</v>
+      </c>
+      <c r="P21" s="51">
+        <v>0.96976806311371933</v>
+      </c>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D22" s="60"/>
+      <c r="E22" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="43">
+        <v>1</v>
+      </c>
+      <c r="I22" s="49">
+        <v>3.7747992514573081E-5</v>
+      </c>
+      <c r="J22" s="50">
+        <v>3.9537071580347435E-5</v>
+      </c>
+      <c r="K22" s="50">
+        <v>3.1040136722672816E-5</v>
+      </c>
+      <c r="L22" s="50">
+        <v>2.2560142302436061E-5</v>
+      </c>
+      <c r="M22" s="50">
+        <v>1.3904588350572295E-5</v>
+      </c>
+      <c r="N22" s="50">
+        <v>6.5737431550899382E-6</v>
+      </c>
+      <c r="O22" s="50">
+        <v>5.6721819182184823E-6</v>
+      </c>
+      <c r="P22" s="51">
+        <v>4.8472784147460675E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D23" s="60"/>
+      <c r="E23" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="43">
+        <v>1</v>
+      </c>
+      <c r="I23" s="49">
+        <v>3.934284519831379E-2</v>
+      </c>
+      <c r="J23" s="50">
+        <v>4.0960406157239941E-2</v>
+      </c>
+      <c r="K23" s="50">
+        <v>3.7724721460420177E-2</v>
+      </c>
+      <c r="L23" s="50">
+        <v>3.5984294670166381E-2</v>
+      </c>
+      <c r="M23" s="50">
+        <v>3.4079328130290895E-2</v>
+      </c>
+      <c r="N23" s="50">
+        <v>3.1145664652910007E-2</v>
+      </c>
+      <c r="O23" s="50">
+        <v>2.7748944186360175E-2</v>
+      </c>
+      <c r="P23" s="51">
+        <v>2.4609632511665785E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D24" s="60"/>
+      <c r="E24" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="43">
+        <v>1</v>
+      </c>
+      <c r="I24" s="49">
+        <v>4.1598287751059542E-3</v>
+      </c>
+      <c r="J24" s="50">
+        <v>3.5005514914599922E-3</v>
+      </c>
+      <c r="K24" s="50">
+        <v>3.1642680553171758E-3</v>
+      </c>
+      <c r="L24" s="50">
+        <v>2.6942016095793833E-3</v>
+      </c>
+      <c r="M24" s="50">
+        <v>2.2754449877230663E-3</v>
+      </c>
+      <c r="N24" s="50">
+        <v>1.9217242490046254E-3</v>
+      </c>
+      <c r="O24" s="50">
+        <v>1.9140462761810593E-3</v>
+      </c>
+      <c r="P24" s="51">
+        <v>1.8969016196372945E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D25" s="60"/>
+      <c r="E25" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="43">
+        <v>1</v>
+      </c>
+      <c r="I25" s="49">
+        <v>6.9173196282955177E-4</v>
+      </c>
+      <c r="J25" s="50">
+        <v>7.0051580671846349E-4</v>
+      </c>
+      <c r="K25" s="50">
+        <v>5.3589883106496894E-4</v>
+      </c>
+      <c r="L25" s="50">
+        <v>3.3406364563222629E-4</v>
+      </c>
+      <c r="M25" s="50">
+        <v>1.5458630577989198E-4</v>
+      </c>
+      <c r="N25" s="50">
+        <v>0</v>
+      </c>
+      <c r="O25" s="50">
+        <v>0</v>
+      </c>
+      <c r="P25" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D26" s="61"/>
+      <c r="E26" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="65">
+        <v>1</v>
+      </c>
+      <c r="I26" s="52">
+        <v>0</v>
+      </c>
+      <c r="J26" s="53">
+        <v>0</v>
+      </c>
+      <c r="K26" s="53">
+        <v>0</v>
+      </c>
+      <c r="L26" s="53">
+        <v>0</v>
+      </c>
+      <c r="M26" s="53">
+        <v>0</v>
+      </c>
+      <c r="N26" s="53">
+        <v>0</v>
+      </c>
+      <c r="O26" s="53">
+        <v>0</v>
+      </c>
+      <c r="P26" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D27" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="59">
+        <v>1</v>
+      </c>
+      <c r="I27" s="45">
+        <v>0.42556332971371874</v>
+      </c>
+      <c r="J27" s="46">
+        <v>0.4387611609386034</v>
+      </c>
+      <c r="K27" s="46">
+        <v>0.44261960515720589</v>
+      </c>
+      <c r="L27" s="46">
+        <v>0.44290296655299799</v>
+      </c>
+      <c r="M27" s="46">
+        <v>0.4365209379689145</v>
+      </c>
+      <c r="N27" s="46">
+        <v>0.41451173512154232</v>
+      </c>
+      <c r="O27" s="46">
+        <v>0.37133349054455705</v>
+      </c>
+      <c r="P27" s="47">
+        <v>0.31861719750149203</v>
+      </c>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D28" s="60"/>
+      <c r="E28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="23">
+        <v>1</v>
+      </c>
+      <c r="I28" s="25">
+        <v>3.9857899708616182E-2</v>
+      </c>
+      <c r="J28" s="26">
+        <v>4.1093997362252291E-2</v>
+      </c>
+      <c r="K28" s="26">
+        <v>4.1455375967875574E-2</v>
+      </c>
+      <c r="L28" s="26">
+        <v>4.1481915355332605E-2</v>
+      </c>
+      <c r="M28" s="26">
+        <v>4.0884179983224668E-2</v>
+      </c>
+      <c r="N28" s="26">
+        <v>3.8822816753579674E-2</v>
+      </c>
+      <c r="O28" s="26">
+        <v>3.4778779070395574E-2</v>
+      </c>
+      <c r="P28" s="48">
+        <v>2.9841415875747242E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D29" s="60"/>
+      <c r="E29" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="43">
+        <v>1</v>
+      </c>
+      <c r="I29" s="49">
+        <v>0.43290649023408723</v>
+      </c>
+      <c r="J29" s="50">
+        <v>0.44270157956346629</v>
+      </c>
+      <c r="K29" s="50">
+        <v>0.43700779627864206</v>
+      </c>
+      <c r="L29" s="50">
+        <v>0.42115097219368908</v>
+      </c>
+      <c r="M29" s="50">
+        <v>0.38398409453487392</v>
+      </c>
+      <c r="N29" s="50">
+        <v>0.32997249939716844</v>
+      </c>
+      <c r="O29" s="50">
+        <v>0.27653309223744926</v>
+      </c>
+      <c r="P29" s="51">
+        <v>0.22563596863358948</v>
+      </c>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D30" s="60"/>
+      <c r="E30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="23">
+        <v>1</v>
+      </c>
+      <c r="I30" s="25">
+        <v>2.4944602281420009E-2</v>
+      </c>
+      <c r="J30" s="26">
+        <v>2.5509007327646552E-2</v>
+      </c>
+      <c r="K30" s="26">
+        <v>2.5180924559842038E-2</v>
+      </c>
+      <c r="L30" s="26">
+        <v>2.4267234931322702E-2</v>
+      </c>
+      <c r="M30" s="26">
+        <v>2.2125633910880578E-2</v>
+      </c>
+      <c r="N30" s="26">
+        <v>1.901341963438264E-2</v>
+      </c>
+      <c r="O30" s="26">
+        <v>1.5934175530111408E-2</v>
+      </c>
+      <c r="P30" s="48">
+        <v>1.3001420918647772E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D31" s="60"/>
+      <c r="E31" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="43">
+        <v>1</v>
+      </c>
+      <c r="I31" s="49">
+        <v>3.638539169699493E-2</v>
+      </c>
+      <c r="J31" s="50">
+        <v>3.500721133687304E-2</v>
+      </c>
+      <c r="K31" s="50">
+        <v>2.9217688019276274E-2</v>
+      </c>
+      <c r="L31" s="50">
+        <v>3.3821014465619852E-2</v>
+      </c>
+      <c r="M31" s="50">
+        <v>5.8599209810369333E-2</v>
+      </c>
+      <c r="N31" s="50">
+        <v>0.10951512246093077</v>
+      </c>
+      <c r="O31" s="50">
+        <v>0.17480089720619413</v>
+      </c>
+      <c r="P31" s="51">
+        <v>0.24365820632430502</v>
+      </c>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D32" s="60"/>
+      <c r="E32" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="43">
+        <v>1</v>
+      </c>
+      <c r="I32" s="49">
+        <v>0.10288236971605716</v>
+      </c>
+      <c r="J32" s="50">
+        <v>8.1917460167846359E-2</v>
+      </c>
+      <c r="K32" s="50">
+        <v>8.9395888673953885E-2</v>
+      </c>
+      <c r="L32" s="50">
+        <v>0.10012790443325413</v>
+      </c>
+      <c r="M32" s="50">
+        <v>0.11834523415808018</v>
+      </c>
+      <c r="N32" s="50">
+        <v>0.14248412543489994</v>
+      </c>
+      <c r="O32" s="50">
+        <v>0.17260530613985245</v>
+      </c>
+      <c r="P32" s="51">
+        <v>0.20606197555747177</v>
+      </c>
+    </row>
+    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D33" s="60"/>
+      <c r="E33" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="41"/>
+      <c r="G33" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="43">
+        <v>1</v>
+      </c>
+      <c r="I33" s="49">
+        <v>5.4111527860738156E-5</v>
+      </c>
+      <c r="J33" s="50">
+        <v>5.3192705911217035E-5</v>
+      </c>
+      <c r="K33" s="50">
+        <v>5.7230300281677974E-5</v>
+      </c>
+      <c r="L33" s="50">
+        <v>9.1081488583802855E-5</v>
+      </c>
+      <c r="M33" s="50">
+        <v>2.9773481638115541E-4</v>
+      </c>
+      <c r="N33" s="50">
+        <v>8.0420604209486852E-4</v>
+      </c>
+      <c r="O33" s="50">
+        <v>1.441441284653545E-3</v>
+      </c>
+      <c r="P33" s="51">
+        <v>2.1041191212510546E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D34" s="60"/>
+      <c r="E34" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="43">
+        <v>1</v>
+      </c>
+      <c r="I34" s="49">
+        <v>1.2957188037907301E-3</v>
+      </c>
+      <c r="J34" s="50">
+        <v>1.5593952872995222E-3</v>
+      </c>
+      <c r="K34" s="50">
+        <v>1.7017915706400845E-3</v>
+      </c>
+      <c r="L34" s="50">
+        <v>1.9060608658553284E-3</v>
+      </c>
+      <c r="M34" s="50">
+        <v>2.2527887113808669E-3</v>
+      </c>
+      <c r="N34" s="50">
+        <v>2.7123115433636854E-3</v>
+      </c>
+      <c r="O34" s="50">
+        <v>3.2857725872935625E-3</v>
+      </c>
+      <c r="P34" s="51">
+        <v>3.9225328618905956E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D35" s="60"/>
+      <c r="E35" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="43">
+        <v>1</v>
+      </c>
+      <c r="I35" s="49">
+        <v>9.1258830749058398E-4</v>
+      </c>
+      <c r="J35" s="50">
+        <v>0</v>
+      </c>
+      <c r="K35" s="50">
+        <v>0</v>
+      </c>
+      <c r="L35" s="50">
+        <v>0</v>
+      </c>
+      <c r="M35" s="50">
+        <v>0</v>
+      </c>
+      <c r="N35" s="50">
+        <v>0</v>
+      </c>
+      <c r="O35" s="50">
+        <v>0</v>
+      </c>
+      <c r="P35" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D36" s="61"/>
+      <c r="E36" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="63"/>
+      <c r="G36" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="65">
+        <v>1</v>
+      </c>
+      <c r="I36" s="52">
+        <v>0</v>
+      </c>
+      <c r="J36" s="53">
+        <v>0</v>
+      </c>
+      <c r="K36" s="53">
+        <v>0</v>
+      </c>
+      <c r="L36" s="53">
+        <v>0</v>
+      </c>
+      <c r="M36" s="53">
+        <v>0</v>
+      </c>
+      <c r="N36" s="53">
+        <v>0</v>
+      </c>
+      <c r="O36" s="53">
+        <v>0</v>
+      </c>
+      <c r="P36" s="54">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429C857E-7E9C-40EC-8492-D79139CDAA51}">
   <dimension ref="B3:P54"/>
   <sheetViews>

</xml_diff>